<commit_message>
chore: update dependencies and code
</commit_message>
<xml_diff>
--- a/TemplateStandalone.xlsx
+++ b/TemplateStandalone.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianzeis/DEV/ui5-cc-excelUpload-sample-standalone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2287BCC9-ABDF-4871-9FB4-FB62248CFB1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F54D987-012C-C441-8060-00B16D4DF6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1605" yWindow="2160" windowWidth="21600" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1600" yWindow="2160" windowWidth="21600" windowHeight="12100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>customer</t>
   </si>
@@ -411,12 +412,12 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -427,7 +428,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -444,4 +445,41 @@
     <ignoredError sqref="A1:C1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12D992F4-F70C-DD4C-84A1-3238A42E8E5E}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>123</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>